<commit_message>
Make changes to LG train model files
</commit_message>
<xml_diff>
--- a/component_warranty_model/Data/LG/unmatched_cases.xlsx
+++ b/component_warranty_model/Data/LG/unmatched_cases.xlsx
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,131 +413,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>text</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>extracted_model</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>reason</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>LG OLED 164CM 65C9</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>No matching spans found or misalignment</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>LG OLED 139cm 55CX</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>No matching spans found or misalignment</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>LG OLED 139cm 55CX</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>No matching spans found or misalignment</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>LG OLED 139cm 55BX</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>No matching spans found or misalignment</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>LG OLED 164CM 65B9</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>No matching spans found or misalignment</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>LG:LED (UHD) TVs:55UQ9000PSD</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>55UQ9000PSD</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>No matching spans found or misalignment</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">55 UN 7300 PTC </t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>55 UN 7300</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>No matching spans found or misalignment</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>